<commit_message>
runpest for icacos works. Set up for calibration of 3 parameters using discharge only.
git-svn-id: svn://136.177.114.72/svn_GW/webmod/trunk@9872 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/projects/PestFiles.xlsx
+++ b/projects/PestFiles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\System\Users\rmwebb\Desktop\webmod\pest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\System\Users\rmwebb\Desktop\webmod\projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -875,7 +876,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F68" sqref="F67:F68"/>
+      <selection pane="bottomRight" activeCell="F67" sqref="F67:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>